<commit_message>
#546 xls script further improvements
</commit_message>
<xml_diff>
--- a/test_suite/test_files/latest/data_summary.xlsx
+++ b/test_suite/test_files/latest/data_summary.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<s:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <s:workbookPr/>
-  <s:bookViews>
-    <s:workbookView activeTab="0"/>
-  </s:bookViews>
-  <s:sheets>
-    <s:sheet name="Sheet" sheetId="1" r:id="rId1"/>
-  </s:sheets>
-  <s:definedNames/>
-  <s:calcPr calcId="124519" fullCalcOnLoad="1"/>
-</s:workbook>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
+  <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\develop\test_suite\test_files\latest\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="12345"/>
+  </bookViews>
+  <sheets>
+    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
+  </sheets>
+  <calcPr calcId="171027"/>
+</workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="76">
   <si>
     <t>PROCESS_run_title</t>
   </si>
@@ -46,6 +51,9 @@
     <t>Electron_temperature_(keV)</t>
   </si>
   <si>
+    <t>Electron_temperature_on_axis_(keV)</t>
+  </si>
+  <si>
     <t>Electron_density_(/m3)</t>
   </si>
   <si>
@@ -82,6 +90,15 @@
     <t>Total_power_lost_due_to_radiation,_ionisation_and_recombination_[W]</t>
   </si>
   <si>
+    <t>Loop_voltage_during_burn_(V)</t>
+  </si>
+  <si>
+    <t>Total_volt-second_requirement_(Wb)</t>
+  </si>
+  <si>
+    <t>Machine_bore_(m)</t>
+  </si>
+  <si>
     <t>CS_radial_thickness_(m)</t>
   </si>
   <si>
@@ -97,6 +114,21 @@
     <t>Axial_stress_in_CS_steel_(Pa)</t>
   </si>
   <si>
+    <t>Electron_temp._at_separatrix_(keV)</t>
+  </si>
+  <si>
+    <t>Electron_density_at_separatrix_(/m3)</t>
+  </si>
+  <si>
+    <t>Pedestal_scaling_switch</t>
+  </si>
+  <si>
+    <t>Electron_temp._pedestal_height_(keV)</t>
+  </si>
+  <si>
+    <t>Electron_density_pedestal_height_(/m3)</t>
+  </si>
+  <si>
     <t>runtitle</t>
   </si>
   <si>
@@ -127,6 +159,9 @@
     <t>te</t>
   </si>
   <si>
+    <t>te0</t>
+  </si>
+  <si>
     <t>dene</t>
   </si>
   <si>
@@ -163,6 +198,15 @@
     <t>totalpowerlost</t>
   </si>
   <si>
+    <t>vburn</t>
+  </si>
+  <si>
+    <t>vsstt</t>
+  </si>
+  <si>
+    <t>bore</t>
+  </si>
+  <si>
     <t>ohcth</t>
   </si>
   <si>
@@ -178,32 +222,59 @@
     <t>sig_axial</t>
   </si>
   <si>
-    <t xml:space="preserve">"Kallenbach divertor model " </t>
+    <t>tesep</t>
+  </si>
+  <si>
+    <t>nesep</t>
+  </si>
+  <si>
+    <t>ieped</t>
+  </si>
+  <si>
+    <t>teped</t>
+  </si>
+  <si>
+    <t>neped</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"EPED scaling with NO corrections " </t>
   </si>
   <si>
     <t>mkovari</t>
   </si>
   <si>
     <t>07/08/2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"0.65 correction factor for teped " </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
-      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -218,17 +289,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -516,21 +598,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:AC3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AL5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="30.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:29">
-      <c r="A1" t="s"/>
+    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <f>SUM(1, 1)</f>
+        <v>2</v>
+      </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -613,184 +697,522 @@
         <v>26</v>
       </c>
       <c r="AC1" t="s">
-        <v>26</v>
+        <v>27</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:29">
-      <c r="A2" t="s"/>
+    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="D2" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="E2" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="F2" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="G2" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="H2" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="I2" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="J2" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="K2" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="L2" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="M2" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="N2" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="O2" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="P2" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="Q2" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="R2" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="S2" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="T2" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="U2" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="V2" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="W2" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="X2" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="Y2" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>70</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>9.2780000000000005</v>
+      </c>
+      <c r="G3">
+        <v>3.1</v>
+      </c>
+      <c r="H3">
+        <v>1978</v>
+      </c>
+      <c r="I3">
+        <v>4.9109999999999996</v>
+      </c>
+      <c r="J3">
+        <v>3.5819999999999998E-2</v>
+      </c>
+      <c r="K3">
+        <v>12.69</v>
+      </c>
+      <c r="L3">
+        <v>25.48</v>
+      </c>
+      <c r="M3">
+        <v>7.239E+19</v>
+      </c>
+      <c r="N3">
+        <v>7.2169999999999998E-2</v>
+      </c>
+      <c r="O3">
+        <v>4.056E+16</v>
+      </c>
+      <c r="P3">
+        <v>302.3</v>
+      </c>
+      <c r="Q3">
+        <v>125.6</v>
+      </c>
+      <c r="R3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="S3">
         <v>50</v>
       </c>
-      <c r="Z2" t="s">
-        <v>51</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>53</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>53</v>
+      <c r="T3">
+        <v>7186</v>
+      </c>
+      <c r="U3">
+        <v>0.48659999999999998</v>
+      </c>
+      <c r="V3">
+        <v>2445000</v>
+      </c>
+      <c r="W3">
+        <v>641900</v>
+      </c>
+      <c r="X3">
+        <v>50640000</v>
+      </c>
+      <c r="Y3">
+        <v>5.0479999999999997E-2</v>
+      </c>
+      <c r="Z3">
+        <v>734.7</v>
+      </c>
+      <c r="AA3">
+        <v>2.4129999999999998</v>
+      </c>
+      <c r="AB3">
+        <v>0.91590000000000005</v>
+      </c>
+      <c r="AC3">
+        <v>0.97829999999999995</v>
+      </c>
+      <c r="AD3">
+        <v>1.5</v>
+      </c>
+      <c r="AE3">
+        <v>249600000</v>
+      </c>
+      <c r="AF3">
+        <v>-350400000</v>
+      </c>
+      <c r="AG3">
+        <v>-350400000</v>
+      </c>
+      <c r="AH3">
+        <v>0.21829999999999999</v>
+      </c>
+      <c r="AI3">
+        <v>3.34E+19</v>
+      </c>
+      <c r="AJ3">
+        <v>1</v>
+      </c>
+      <c r="AK3">
+        <v>6</v>
+      </c>
+      <c r="AL3">
+        <v>5.679E+19</v>
       </c>
     </row>
-    <row r="3" spans="1:29">
-      <c r="A3" t="s"/>
-      <c r="B3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E3" t="n">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E4">
         <v>1</v>
       </c>
-      <c r="F3" t="n">
-        <v>9.257999999999999</v>
-      </c>
-      <c r="G3" t="n">
+      <c r="F4">
+        <v>9.1769999999999996</v>
+      </c>
+      <c r="G4">
         <v>3.1</v>
       </c>
-      <c r="H3" t="n">
-        <v>1976</v>
-      </c>
-      <c r="I3" t="n">
-        <v>4.902</v>
-      </c>
-      <c r="J3" t="n">
-        <v>0.03588</v>
-      </c>
-      <c r="K3" t="n">
-        <v>12.6</v>
-      </c>
-      <c r="L3" t="n">
-        <v>7.241e+19</v>
-      </c>
-      <c r="M3" t="n">
-        <v>0.07201</v>
-      </c>
-      <c r="N3" t="n">
-        <v>4.041e+16</v>
-      </c>
-      <c r="O3" t="n">
-        <v>302.9</v>
-      </c>
-      <c r="P3" t="n">
-        <v>124.6</v>
-      </c>
-      <c r="Q3" t="n">
-        <v>1.1</v>
-      </c>
-      <c r="R3" t="n">
+      <c r="H4">
+        <v>1969</v>
+      </c>
+      <c r="I4">
+        <v>4.867</v>
+      </c>
+      <c r="J4">
+        <v>3.6130000000000002E-2</v>
+      </c>
+      <c r="K4">
+        <v>12.31</v>
+      </c>
+      <c r="L4">
+        <v>27.87</v>
+      </c>
+      <c r="M4">
+        <v>7.254E+19</v>
+      </c>
+      <c r="N4">
+        <v>7.1300000000000002E-2</v>
+      </c>
+      <c r="O4">
+        <v>3.965E+16</v>
+      </c>
+      <c r="P4">
+        <v>305.5</v>
+      </c>
+      <c r="Q4">
+        <v>120.7</v>
+      </c>
+      <c r="R4">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="S4">
         <v>50</v>
       </c>
-      <c r="S3" t="n">
+      <c r="T4">
         <v>7186</v>
       </c>
-      <c r="T3" t="n">
-        <v>0.4866</v>
-      </c>
-      <c r="U3" t="n">
-        <v>2437000</v>
-      </c>
-      <c r="V3" t="n">
-        <v>640600</v>
-      </c>
-      <c r="W3" t="n">
-        <v>50260000</v>
-      </c>
-      <c r="X3" t="n">
-        <v>0.9131</v>
-      </c>
-      <c r="Y3" t="n">
-        <v>0.9741</v>
-      </c>
-      <c r="Z3" t="n">
+      <c r="U4">
+        <v>0.48620000000000002</v>
+      </c>
+      <c r="V4">
+        <v>2400000</v>
+      </c>
+      <c r="W4">
+        <v>635200</v>
+      </c>
+      <c r="X4">
+        <v>48610000</v>
+      </c>
+      <c r="Y4">
+        <v>4.9160000000000002E-2</v>
+      </c>
+      <c r="Z4">
+        <v>713.8</v>
+      </c>
+      <c r="AA4">
+        <v>2.3780000000000001</v>
+      </c>
+      <c r="AB4">
+        <v>0.90129999999999999</v>
+      </c>
+      <c r="AC4">
+        <v>0.95909999999999995</v>
+      </c>
+      <c r="AD4">
         <v>1.5</v>
       </c>
-      <c r="AA3" t="n">
-        <v>249900000</v>
-      </c>
-      <c r="AB3" t="n">
-        <v>-350100000</v>
-      </c>
-      <c r="AC3" t="n">
-        <v>-350100000</v>
+      <c r="AE4">
+        <v>251000000</v>
+      </c>
+      <c r="AF4">
+        <v>-349000000</v>
+      </c>
+      <c r="AG4">
+        <v>-349000000</v>
+      </c>
+      <c r="AH4">
+        <v>0.21560000000000001</v>
+      </c>
+      <c r="AI4">
+        <v>3.347E+19</v>
+      </c>
+      <c r="AJ4">
+        <v>1</v>
+      </c>
+      <c r="AK4">
+        <v>3.8730000000000002</v>
+      </c>
+      <c r="AL4">
+        <v>5.69E+19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="F5" s="1">
+        <f>F4/F3-1</f>
+        <v>-1.0885966803190428E-2</v>
+      </c>
+      <c r="G5" s="1">
+        <f t="shared" ref="G5:AL5" si="0">G4/G3-1</f>
+        <v>0</v>
+      </c>
+      <c r="H5" s="1">
+        <f t="shared" si="0"/>
+        <v>-4.5500505561172355E-3</v>
+      </c>
+      <c r="I5" s="1">
+        <f t="shared" si="0"/>
+        <v>-8.9594787212379234E-3</v>
+      </c>
+      <c r="J5" s="1">
+        <f t="shared" si="0"/>
+        <v>8.6543830262424404E-3</v>
+      </c>
+      <c r="K5" s="1">
+        <f t="shared" si="0"/>
+        <v>-2.9944838455476686E-2</v>
+      </c>
+      <c r="L5" s="1">
+        <f t="shared" si="0"/>
+        <v>9.3799058084772291E-2</v>
+      </c>
+      <c r="M5" s="1">
+        <f t="shared" si="0"/>
+        <v>2.0721094073767876E-3</v>
+      </c>
+      <c r="N5" s="1">
+        <f t="shared" si="0"/>
+        <v>-1.2054870444783039E-2</v>
+      </c>
+      <c r="O5" s="1">
+        <f t="shared" si="0"/>
+        <v>-2.2435897435897467E-2</v>
+      </c>
+      <c r="P5" s="1">
+        <f t="shared" si="0"/>
+        <v>1.05855110817068E-2</v>
+      </c>
+      <c r="Q5" s="1">
+        <f t="shared" si="0"/>
+        <v>-3.9012738853503093E-2</v>
+      </c>
+      <c r="R5" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="S5" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="T5" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U5" s="1">
+        <f t="shared" si="0"/>
+        <v>-8.2203041512529662E-4</v>
+      </c>
+      <c r="V5" s="1">
+        <f t="shared" si="0"/>
+        <v>-1.8404907975460127E-2</v>
+      </c>
+      <c r="W5" s="1">
+        <f t="shared" si="0"/>
+        <v>-1.0437762891416069E-2</v>
+      </c>
+      <c r="X5" s="1">
+        <f t="shared" si="0"/>
+        <v>-4.0086887835703022E-2</v>
+      </c>
+      <c r="Y5" s="1">
+        <f t="shared" si="0"/>
+        <v>-2.6148969889064899E-2</v>
+      </c>
+      <c r="Z5" s="1">
+        <f t="shared" si="0"/>
+        <v>-2.8446985164012673E-2</v>
+      </c>
+      <c r="AA5" s="1">
+        <f t="shared" si="0"/>
+        <v>-1.4504765851636847E-2</v>
+      </c>
+      <c r="AB5" s="1">
+        <f t="shared" si="0"/>
+        <v>-1.5940604869527308E-2</v>
+      </c>
+      <c r="AC5" s="1">
+        <f t="shared" si="0"/>
+        <v>-1.9625881631401443E-2</v>
+      </c>
+      <c r="AD5" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AE5" s="1">
+        <f t="shared" si="0"/>
+        <v>5.6089743589744501E-3</v>
+      </c>
+      <c r="AF5" s="1">
+        <f t="shared" si="0"/>
+        <v>-3.9954337899543724E-3</v>
+      </c>
+      <c r="AG5" s="1">
+        <f t="shared" si="0"/>
+        <v>-3.9954337899543724E-3</v>
+      </c>
+      <c r="AH5" s="1">
+        <f t="shared" si="0"/>
+        <v>-1.2368300503893592E-2</v>
+      </c>
+      <c r="AI5" s="1">
+        <f t="shared" si="0"/>
+        <v>2.0958083832336438E-3</v>
+      </c>
+      <c r="AJ5" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AK5" s="1">
+        <f t="shared" si="0"/>
+        <v>-0.35449999999999993</v>
+      </c>
+      <c r="AL5" s="1">
+        <f t="shared" si="0"/>
+        <v>1.9369607325232518E-3</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <conditionalFormatting sqref="F5:AJ5">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
2-phase quench model: phase 1 completed - Issue #548
</commit_message>
<xml_diff>
--- a/test_suite/test_files/latest/data_summary.xlsx
+++ b/test_suite/test_files/latest/data_summary.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="78">
   <si>
     <t>PROCESS_run_title</t>
   </si>
@@ -247,6 +247,12 @@
   </si>
   <si>
     <t xml:space="preserve">"0.65 correction factor for teped " </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"EPED scaling OFF. teped=5.5 keV " </t>
+  </si>
+  <si>
+    <t>08/08/2017</t>
   </si>
 </sst>
 </file>
@@ -256,14 +262,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -289,17 +288,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -599,22 +596,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AL5"/>
+  <dimension ref="B1:AL8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <f>SUM(1, 1)</f>
-        <v>2</v>
-      </c>
+    <row r="1" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -727,7 +718,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>36</v>
       </c>
@@ -840,7 +831,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>72</v>
       </c>
@@ -953,7 +944,7 @@
         <v>5.679E+19</v>
       </c>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>75</v>
       </c>
@@ -1066,13 +1057,9 @@
         <v>5.69E+19</v>
       </c>
     </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="F5" s="1">
-        <f>F4/F3-1</f>
-        <v>-1.0885966803190428E-2</v>
-      </c>
+    <row r="5" spans="2:38" x14ac:dyDescent="0.25">
       <c r="G5" s="1">
-        <f t="shared" ref="G5:AL5" si="0">G4/G3-1</f>
+        <f t="shared" ref="F5:AL5" si="0">G4/G3-1</f>
         <v>0</v>
       </c>
       <c r="H5" s="1">
@@ -1198,10 +1185,370 @@
       <c r="AL5" s="1">
         <f t="shared" si="0"/>
         <v>1.9369607325232518E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" t="s">
+        <v>41</v>
+      </c>
+      <c r="H6" t="s">
+        <v>42</v>
+      </c>
+      <c r="I6" t="s">
+        <v>43</v>
+      </c>
+      <c r="J6" t="s">
+        <v>44</v>
+      </c>
+      <c r="K6" t="s">
+        <v>45</v>
+      </c>
+      <c r="L6" t="s">
+        <v>46</v>
+      </c>
+      <c r="M6" t="s">
+        <v>47</v>
+      </c>
+      <c r="N6" t="s">
+        <v>48</v>
+      </c>
+      <c r="O6" t="s">
+        <v>49</v>
+      </c>
+      <c r="P6" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>51</v>
+      </c>
+      <c r="R6" t="s">
+        <v>52</v>
+      </c>
+      <c r="S6" t="s">
+        <v>53</v>
+      </c>
+      <c r="T6" t="s">
+        <v>54</v>
+      </c>
+      <c r="U6" t="s">
+        <v>55</v>
+      </c>
+      <c r="V6" t="s">
+        <v>56</v>
+      </c>
+      <c r="W6" t="s">
+        <v>57</v>
+      </c>
+      <c r="X6" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>65</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>66</v>
+      </c>
+      <c r="AG6" t="s">
+        <v>66</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>67</v>
+      </c>
+      <c r="AI6" t="s">
+        <v>68</v>
+      </c>
+      <c r="AJ6" t="s">
+        <v>69</v>
+      </c>
+      <c r="AK6" t="s">
+        <v>70</v>
+      </c>
+      <c r="AL6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D7" t="s">
+        <v>77</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>9.2579999999999991</v>
+      </c>
+      <c r="G7">
+        <v>3.1</v>
+      </c>
+      <c r="H7">
+        <v>1976</v>
+      </c>
+      <c r="I7">
+        <v>4.9020000000000001</v>
+      </c>
+      <c r="J7">
+        <v>3.5880000000000002E-2</v>
+      </c>
+      <c r="K7">
+        <v>12.6</v>
+      </c>
+      <c r="L7">
+        <v>26.05</v>
+      </c>
+      <c r="M7">
+        <v>7.241E+19</v>
+      </c>
+      <c r="N7">
+        <v>7.2010000000000005E-2</v>
+      </c>
+      <c r="O7">
+        <v>4.041E+16</v>
+      </c>
+      <c r="P7">
+        <v>302.89999999999998</v>
+      </c>
+      <c r="Q7">
+        <v>124.6</v>
+      </c>
+      <c r="R7">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="S7">
+        <v>50</v>
+      </c>
+      <c r="T7">
+        <v>7186</v>
+      </c>
+      <c r="U7">
+        <v>0.48659999999999998</v>
+      </c>
+      <c r="V7">
+        <v>2437000</v>
+      </c>
+      <c r="W7">
+        <v>640600</v>
+      </c>
+      <c r="X7">
+        <v>50260000</v>
+      </c>
+      <c r="Y7">
+        <v>5.024E-2</v>
+      </c>
+      <c r="Z7">
+        <v>730.6</v>
+      </c>
+      <c r="AA7">
+        <v>2.4060000000000001</v>
+      </c>
+      <c r="AB7">
+        <v>0.91310000000000002</v>
+      </c>
+      <c r="AC7">
+        <v>0.97409999999999997</v>
+      </c>
+      <c r="AD7">
+        <v>1.5</v>
+      </c>
+      <c r="AE7">
+        <v>249900000</v>
+      </c>
+      <c r="AF7">
+        <v>-350100000</v>
+      </c>
+      <c r="AG7">
+        <v>-350100000</v>
+      </c>
+      <c r="AH7">
+        <v>0.21779999999999999</v>
+      </c>
+      <c r="AI7">
+        <v>3.341E+19</v>
+      </c>
+      <c r="AJ7">
+        <v>0</v>
+      </c>
+      <c r="AK7">
+        <v>5.5</v>
+      </c>
+      <c r="AL7">
+        <v>5.68E+19</v>
+      </c>
+    </row>
+    <row r="8" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="F8" s="1">
+        <f>F7/F3-1</f>
+        <v>-2.155636990730958E-3</v>
+      </c>
+      <c r="G8" s="1">
+        <f t="shared" ref="G8:AL8" si="1">G7/G3-1</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="1">
+        <f t="shared" si="1"/>
+        <v>-1.0111223458038054E-3</v>
+      </c>
+      <c r="I8" s="1">
+        <f t="shared" si="1"/>
+        <v>-1.8326206475258733E-3</v>
+      </c>
+      <c r="J8" s="1">
+        <f t="shared" si="1"/>
+        <v>1.6750418760469454E-3</v>
+      </c>
+      <c r="K8" s="1">
+        <f t="shared" si="1"/>
+        <v>-7.0921985815602939E-3</v>
+      </c>
+      <c r="L8" s="1">
+        <f t="shared" si="1"/>
+        <v>2.2370486656200894E-2</v>
+      </c>
+      <c r="M8" s="1">
+        <f t="shared" si="1"/>
+        <v>2.7628125431689021E-4</v>
+      </c>
+      <c r="N8" s="1">
+        <f t="shared" si="1"/>
+        <v>-2.216987668006043E-3</v>
+      </c>
+      <c r="O8" s="1">
+        <f t="shared" si="1"/>
+        <v>-3.6982248520710526E-3</v>
+      </c>
+      <c r="P8" s="1">
+        <f t="shared" si="1"/>
+        <v>1.9847833278199278E-3</v>
+      </c>
+      <c r="Q8" s="1">
+        <f t="shared" si="1"/>
+        <v>-7.9617834394904996E-3</v>
+      </c>
+      <c r="R8" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S8" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T8" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="U8" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="V8" s="1">
+        <f t="shared" si="1"/>
+        <v>-3.2719836400818547E-3</v>
+      </c>
+      <c r="W8" s="1">
+        <f t="shared" si="1"/>
+        <v>-2.0252375759464147E-3</v>
+      </c>
+      <c r="X8" s="1">
+        <f t="shared" si="1"/>
+        <v>-7.5039494470774404E-3</v>
+      </c>
+      <c r="Y8" s="1">
+        <f t="shared" si="1"/>
+        <v>-4.7543581616481534E-3</v>
+      </c>
+      <c r="Z8" s="1">
+        <f t="shared" si="1"/>
+        <v>-5.5805090513134648E-3</v>
+      </c>
+      <c r="AA8" s="1">
+        <f t="shared" si="1"/>
+        <v>-2.9009531703272362E-3</v>
+      </c>
+      <c r="AB8" s="1">
+        <f t="shared" si="1"/>
+        <v>-3.0571023037450074E-3</v>
+      </c>
+      <c r="AC8" s="1">
+        <f t="shared" si="1"/>
+        <v>-4.2931616068689893E-3</v>
+      </c>
+      <c r="AD8" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AE8" s="1">
+        <f t="shared" si="1"/>
+        <v>1.2019230769231282E-3</v>
+      </c>
+      <c r="AF8" s="1">
+        <f t="shared" si="1"/>
+        <v>-8.561643835616195E-4</v>
+      </c>
+      <c r="AG8" s="1">
+        <f t="shared" si="1"/>
+        <v>-8.561643835616195E-4</v>
+      </c>
+      <c r="AH8" s="1">
+        <f t="shared" si="1"/>
+        <v>-2.2904260192395665E-3</v>
+      </c>
+      <c r="AI8" s="1">
+        <f t="shared" si="1"/>
+        <v>2.9940119760474282E-4</v>
+      </c>
+      <c r="AJ8" s="1">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+      <c r="AK8" s="1">
+        <f t="shared" si="1"/>
+        <v>-8.333333333333337E-2</v>
+      </c>
+      <c r="AL8" s="1">
+        <f t="shared" si="1"/>
+        <v>1.7608733932039655E-4</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="F5:AJ5">
+  <conditionalFormatting sqref="G5:AJ5 F8:AL8">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>